<commit_message>
added Byss-Calle removed redundant file names from project directory
</commit_message>
<xml_diff>
--- a/Nyckelharpa_Origins/NyckelharpaHistoryData.xlsx
+++ b/Nyckelharpa_Origins/NyckelharpaHistoryData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiadso\Documents\R\Nyckelharpa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiadso\Documents\R\Nyckelharpa\Nyckelharpa_Origins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68DC2E83-1C61-4FEA-AD26-D7F57DC3DC2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBD99FC-0BE5-461A-8371-F18DAC484386}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{98133621-DC91-4BD8-89EA-20271672BCB4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="147">
   <si>
     <t>InstrumentName</t>
   </si>
@@ -362,51 +362,6 @@
     <t>Sandberg, Paul/Upplandsmuseet</t>
   </si>
   <si>
-    <t>www/images/kallunge_carving.jpg</t>
-  </si>
-  <si>
-    <t>www/images/moraharpa.jpg</t>
-  </si>
-  <si>
-    <t>www/images/vefsen.png</t>
-  </si>
-  <si>
-    <t>www/images/esse_harpa.jpg</t>
-  </si>
-  <si>
-    <t>www/images/kontrabasharpa.jpg</t>
-  </si>
-  <si>
-    <t>www/images/sigtuna.jpg</t>
-  </si>
-  <si>
-    <t>www/images/ESI.jpg</t>
-  </si>
-  <si>
-    <t>www/images/Viola_a_chiavi_Siena_1408.jpg</t>
-  </si>
-  <si>
-    <t>www/images/tolfta.jpg</t>
-  </si>
-  <si>
-    <t>www/images/Schluesselfidel.jpg</t>
-  </si>
-  <si>
-    <t>www/images/Strohfiddel.jpg</t>
-  </si>
-  <si>
-    <t>www/images/Silverbasharpa.jpg</t>
-  </si>
-  <si>
-    <t>www/images/lagga-600.jpg</t>
-  </si>
-  <si>
-    <t>www/images/eric.jpg</t>
-  </si>
-  <si>
-    <t>www/images/bohlin.jpeg</t>
-  </si>
-  <si>
     <t>RemoteImage</t>
   </si>
   <si>
@@ -453,6 +408,72 @@
   </si>
   <si>
     <t>https://reportingnotes.com/wp-content/uploads/2019/05/Viola_a_chiavi_Siena_1408.jpg</t>
+  </si>
+  <si>
+    <t>Älvkarleby</t>
+  </si>
+  <si>
+    <t>1800 CE</t>
+  </si>
+  <si>
+    <t>http://matscarlsson.eu/familj/pdf/byss-calle.pdf</t>
+  </si>
+  <si>
+    <t>bysscalle.png</t>
+  </si>
+  <si>
+    <t>kallunge_carving.jpg</t>
+  </si>
+  <si>
+    <t>moraharpa.jpg</t>
+  </si>
+  <si>
+    <t>vefsen.png</t>
+  </si>
+  <si>
+    <t>esse_harpa.jpg</t>
+  </si>
+  <si>
+    <t>kontrabasharpa.jpg</t>
+  </si>
+  <si>
+    <t>sigtuna.jpg</t>
+  </si>
+  <si>
+    <t>ESI.jpg</t>
+  </si>
+  <si>
+    <t>Viola_a_chiavi_Siena_1408.jpg</t>
+  </si>
+  <si>
+    <t>tolfta.jpg</t>
+  </si>
+  <si>
+    <t>Schluesselfidel.jpg</t>
+  </si>
+  <si>
+    <t>Strohfiddel.jpg</t>
+  </si>
+  <si>
+    <t>Silverbasharpa.jpg</t>
+  </si>
+  <si>
+    <t>lagga-600.jpg</t>
+  </si>
+  <si>
+    <t>eric.jpg</t>
+  </si>
+  <si>
+    <t>bohlin.jpeg</t>
+  </si>
+  <si>
+    <t>https://reportingnotes.com/wp-content/uploads/2019/05/byssecalle.png</t>
+  </si>
+  <si>
+    <t>public domain, drawing by Olaf Thunman</t>
+  </si>
+  <si>
+    <t>Bysse-Calle was a prolific composer of nyckelharpa tunes, and played at a lot of weddings.</t>
   </si>
 </sst>
 </file>
@@ -853,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C19648A-7D51-4B77-BA95-465F033E890E}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +917,7 @@
         <v>64</v>
       </c>
       <c r="I1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="J1" t="s">
         <v>66</v>
@@ -925,10 +946,10 @@
         <v>63</v>
       </c>
       <c r="H2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
         <v>104</v>
@@ -957,10 +978,10 @@
         <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="I3" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="J3" t="s">
         <v>104</v>
@@ -989,10 +1010,10 @@
         <v>61</v>
       </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
       <c r="I4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
         <v>104</v>
@@ -1021,10 +1042,10 @@
         <v>50</v>
       </c>
       <c r="H5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" t="s">
         <v>112</v>
-      </c>
-      <c r="I5" t="s">
-        <v>127</v>
       </c>
       <c r="J5" t="s">
         <v>103</v>
@@ -1053,10 +1074,10 @@
         <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="I6" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="J6" t="s">
         <v>103</v>
@@ -1085,10 +1106,10 @@
         <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="I7" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="J7" t="s">
         <v>78</v>
@@ -1117,10 +1138,10 @@
         <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="I8" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="J8" t="s">
         <v>93</v>
@@ -1149,10 +1170,10 @@
         <v>51</v>
       </c>
       <c r="H9" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="I9" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="J9" t="s">
         <v>81</v>
@@ -1181,10 +1202,10 @@
         <v>55</v>
       </c>
       <c r="H10" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="I10" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="J10" t="s">
         <v>80</v>
@@ -1213,10 +1234,10 @@
         <v>58</v>
       </c>
       <c r="H11" t="s">
+        <v>138</v>
+      </c>
+      <c r="I11" t="s">
         <v>118</v>
-      </c>
-      <c r="I11" t="s">
-        <v>133</v>
       </c>
       <c r="J11" t="s">
         <v>80</v>
@@ -1245,10 +1266,10 @@
         <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="I12" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="J12" t="s">
         <v>80</v>
@@ -1277,10 +1298,10 @@
         <v>86</v>
       </c>
       <c r="H13" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" t="s">
         <v>120</v>
-      </c>
-      <c r="I13" t="s">
-        <v>135</v>
       </c>
       <c r="J13" t="s">
         <v>89</v>
@@ -1309,10 +1330,10 @@
         <v>86</v>
       </c>
       <c r="H14" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="I14" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="J14" t="s">
         <v>89</v>
@@ -1341,10 +1362,10 @@
         <v>91</v>
       </c>
       <c r="H15" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>91</v>
@@ -1373,17 +1394,49 @@
         <v>107</v>
       </c>
       <c r="H16" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="I16" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="J16" t="s">
         <v>108</v>
       </c>
     </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17">
+        <v>60.571396900000003</v>
+      </c>
+      <c r="D17">
+        <v>17.412947200000001</v>
+      </c>
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="F17" t="s">
+        <v>146</v>
+      </c>
+      <c r="G17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J17" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:D1048576">
+  <conditionalFormatting sqref="C19:D1048576 D18 C1:D17">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
@@ -1393,9 +1446,10 @@
     <hyperlink ref="J15" r:id="rId4" xr:uid="{D903E0E2-55F0-4FE3-9145-7D7D150CDADC}"/>
     <hyperlink ref="G6" r:id="rId5" xr:uid="{F17BAB83-F487-4B2C-B3F5-33A282756CFF}"/>
     <hyperlink ref="G3" r:id="rId6" xr:uid="{7C81E384-367B-4916-9C3C-C806804FF5E1}"/>
+    <hyperlink ref="I17" r:id="rId7" xr:uid="{613DDF59-9E45-4CC2-ABCB-AD00DA0A242A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>